<commit_message>
Final Update Done !
</commit_message>
<xml_diff>
--- a/app/data/new_trade_log.xlsx
+++ b/app/data/new_trade_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanju\Documents\EchoEphemeris\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D169F0-037A-46CF-914B-29C352B713C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8BF52B-7BD1-42ED-A0D7-A5B0D1F8FBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{64A77041-B254-4548-9B62-F2D024C124CE}"/>
   </bookViews>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DB8981-B981-45E6-869B-39E0DF2F3D78}">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,6 +1144,7 @@
         <v>60</v>
       </c>
       <c r="K2">
+        <f>-(I2*J2)</f>
         <v>-1500</v>
       </c>
       <c r="L2" s="1">
@@ -1165,7 +1166,7 @@
         <v>1605</v>
       </c>
       <c r="S2">
-        <f>R2+K2</f>
+        <f t="shared" ref="S2:S9" si="0">R2+K2</f>
         <v>105</v>
       </c>
     </row>
@@ -1198,6 +1199,7 @@
         <v>178.7</v>
       </c>
       <c r="K3">
+        <f>-(I3*J3)</f>
         <v>-8935</v>
       </c>
       <c r="L3" s="1">
@@ -1220,7 +1222,7 @@
         <v>9365</v>
       </c>
       <c r="S3">
-        <f>R3+K3</f>
+        <f t="shared" si="0"/>
         <v>430</v>
       </c>
     </row>
@@ -1253,7 +1255,8 @@
         <v>196.18</v>
       </c>
       <c r="K4">
-        <v>-2942.75</v>
+        <f>-(I4*J4)</f>
+        <v>-2942.7000000000003</v>
       </c>
       <c r="L4" s="1">
         <v>45471</v>
@@ -1274,8 +1277,8 @@
         <v>3355.05</v>
       </c>
       <c r="S4">
-        <f>R4+K4</f>
-        <v>412.30000000000018</v>
+        <f t="shared" si="0"/>
+        <v>412.34999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1307,6 +1310,7 @@
         <v>142.15</v>
       </c>
       <c r="K5">
+        <f>-(I5*J5)</f>
         <v>-3553.75</v>
       </c>
       <c r="L5" s="1">
@@ -1328,7 +1332,7 @@
         <v>3730</v>
       </c>
       <c r="S5">
-        <f>R5+K5</f>
+        <f t="shared" si="0"/>
         <v>176.25</v>
       </c>
     </row>
@@ -1361,7 +1365,8 @@
         <v>298.08</v>
       </c>
       <c r="K6">
-        <v>-8942.5</v>
+        <f>-(I6*J6)</f>
+        <v>-8942.4</v>
       </c>
       <c r="L6" s="1">
         <v>45474</v>
@@ -1382,8 +1387,8 @@
         <v>9523.2000000000007</v>
       </c>
       <c r="S6">
-        <f>R6+K6</f>
-        <v>580.70000000000073</v>
+        <f t="shared" si="0"/>
+        <v>580.80000000000109</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1415,7 +1420,8 @@
         <v>131.97999999999999</v>
       </c>
       <c r="K7">
-        <v>-1979.75</v>
+        <f>-(I7*J7)</f>
+        <v>-1979.6999999999998</v>
       </c>
       <c r="L7" s="1">
         <v>45475</v>
@@ -1436,8 +1442,8 @@
         <v>1458.3</v>
       </c>
       <c r="S7">
-        <f>R7+K7</f>
-        <v>-521.45000000000005</v>
+        <f t="shared" si="0"/>
+        <v>-521.39999999999986</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1469,6 +1475,7 @@
         <v>92.95</v>
       </c>
       <c r="K8">
+        <f>-(I8*J8)</f>
         <v>-2323.75</v>
       </c>
       <c r="L8" s="1">
@@ -1490,7 +1497,7 @@
         <v>1441.25</v>
       </c>
       <c r="S8">
-        <f>R8+K8</f>
+        <f t="shared" si="0"/>
         <v>-882.5</v>
       </c>
     </row>
@@ -1523,6 +1530,7 @@
         <v>374.08</v>
       </c>
       <c r="K9">
+        <f>-(I9*J9)</f>
         <v>-28056</v>
       </c>
       <c r="L9" s="1">
@@ -1545,7 +1553,7 @@
         <v>30000</v>
       </c>
       <c r="S9">
-        <f>R9+K9</f>
+        <f t="shared" si="0"/>
         <v>1944</v>
       </c>
     </row>

</xml_diff>